<commit_message>
Update to section metadata
Corrected error in Section_name column for sample P11

P11_1_A to P11_1_A
P11_1_A to P11_2_A
P11_1_A to P11_3_A
P11_1_A to P11_4_A
P11_1_A to P11_5_A
P11_1_A to P11_6_A
P11_1_A to P11_7_A
P11_1_A to P11_8_A
</commit_message>
<xml_diff>
--- a/Section_data_plus_metadata.xlsx
+++ b/Section_data_plus_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kansas-my.sharepoint.com/personal/j853s117_home_ku_edu/Documents/Wagner Postdoc/Tripsacum_Water_Stress_Anatomy/GITHUB/Tripsacum-dactyloides-Root-Anatomical-Responses-to-Drought-and-Waterlogging/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="354" documentId="11_E9DA91FD927742E11418645EFE117A28C07F1320" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA812282-0B86-4A9D-BBE2-0FE2C4BF1EC3}"/>
+  <xr:revisionPtr revIDLastSave="361" documentId="11_E9DA91FD927742E11418645EFE117A28C07F1320" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81DCF690-04E2-4E70-B869-D4755D27696B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="507" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3083" uniqueCount="1282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3083" uniqueCount="1289">
   <si>
     <t>Treatment</t>
   </si>
@@ -3882,6 +3882,27 @@
   </si>
   <si>
     <t>P09_8_A</t>
+  </si>
+  <si>
+    <t>P11_2_A</t>
+  </si>
+  <si>
+    <t>P11_3_A</t>
+  </si>
+  <si>
+    <t>P11_4_A</t>
+  </si>
+  <si>
+    <t>P11_5_A</t>
+  </si>
+  <si>
+    <t>P11_6_A</t>
+  </si>
+  <si>
+    <t>P11_7_A</t>
+  </si>
+  <si>
+    <t>P11_8_A</t>
   </si>
 </sst>
 </file>
@@ -4101,7 +4122,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4110,10 +4131,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -4416,8 +4437,8 @@
   <dimension ref="A1:P606"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8345,7 +8366,7 @@
         <v>1175</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>1176</v>
+        <v>1282</v>
       </c>
       <c r="C79" s="9">
         <v>2</v>
@@ -8395,7 +8416,7 @@
         <v>1175</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>1176</v>
+        <v>1283</v>
       </c>
       <c r="C80" s="9">
         <v>3</v>
@@ -8445,7 +8466,7 @@
         <v>1175</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>1176</v>
+        <v>1284</v>
       </c>
       <c r="C81" s="9">
         <v>4</v>
@@ -8495,7 +8516,7 @@
         <v>1175</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>1176</v>
+        <v>1285</v>
       </c>
       <c r="C82" s="9">
         <v>5</v>
@@ -8545,7 +8566,7 @@
         <v>1175</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>1176</v>
+        <v>1286</v>
       </c>
       <c r="C83" s="9">
         <v>6</v>
@@ -8595,7 +8616,7 @@
         <v>1175</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>1176</v>
+        <v>1287</v>
       </c>
       <c r="C84" s="9">
         <v>7</v>
@@ -8645,7 +8666,7 @@
         <v>1175</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>1176</v>
+        <v>1288</v>
       </c>
       <c r="C85" s="9">
         <v>8</v>

</xml_diff>